<commit_message>
updated web service func
</commit_message>
<xml_diff>
--- a/assets/translate_prompt.xlsx
+++ b/assets/translate_prompt.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>type</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>VI</t>
-  </si>
-  <si>
-    <t>acc</t>
   </si>
   <si>
     <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
@@ -104,9 +101,6 @@
 {text}</t>
   </si>
   <si>
-    <t>loose</t>
-  </si>
-  <si>
     <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
 Hãy chuyển ngữ văn bản sau đây từ tiếng Trung sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
 {count_info} 
@@ -243,9 +237,6 @@
 Vẫn giữ định dạng đánh số và cấu trúc đoạn văn như bản gốc (1., 2., ...)
 Đây là văn bản cần chuyển ngữ:
 {text}</t>
-  </si>
-  <si>
-    <t>cho bộ ORV từ tiếng Trung</t>
   </si>
   <si>
     <t>You are a master literary translator and accomplished author with decades of experience in both Vietnamese and English literature. Your translations read as if originally written by a native English-speaking novelist.
@@ -272,6 +263,15 @@
   </si>
   <si>
     <t>Custom</t>
+  </si>
+  <si>
+    <t>JP_acc</t>
+  </si>
+  <si>
+    <t>JP_loose</t>
+  </si>
+  <si>
+    <t>KR_loose</t>
   </si>
 </sst>
 </file>
@@ -664,8 +664,8 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,57 +699,57 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -757,29 +757,29 @@
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -789,29 +789,27 @@
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G8" s="5"/>
     </row>

</xml_diff>

<commit_message>
fixed JP epub converter
</commit_message>
<xml_diff>
--- a/assets/translate_prompt.xlsx
+++ b/assets/translate_prompt.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Python\AI_Translation_Bridge\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>type</t>
   </si>
@@ -56,15 +61,6 @@
   </si>
   <si>
     <t>Custom</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
   </si>
   <si>
     <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
@@ -130,12 +126,6 @@
 Đối với tên nhân vật, hãy chuyển sang phát âm tiếng Nhật, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
 Bạn có thể điều chỉnh cấu trúc câu để tạo nhịp điệu đọc tốt hơn, miễn là không làm mất ý nghĩa gốc.
 Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản.</t>
-  </si>
-  <si>
-    <t>ggggaaaffaafattrr</t>
-  </si>
-  <si>
-    <t>bbbxxx</t>
   </si>
   <si>
     <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các tác phẩm văn học tiếng Anh sang tiếng Việt. 
@@ -241,15 +231,12 @@
   <si>
     <t>Custom Prompt</t>
   </si>
-  <si>
-    <t>a</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +299,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -358,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,9 +385,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,6 +420,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -599,14 +596,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,141 +628,111 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>